<commit_message>
Latest update_Commit_11-Jan-23 - Jose
</commit_message>
<xml_diff>
--- a/Requirements/Requirments_v6.0.xlsx
+++ b/Requirements/Requirments_v6.0.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
   <si>
     <t>Capture Commodity details - Add in Gate-In Form (Change Stock Type to Commodity Type) (Garments, Auto Parts, Leather Garments, Shoe Uppers, Finish Leather, Console, Electrical &amp; Electronics) - Jose (Venkat to send commodity details list)</t>
   </si>
@@ -230,6 +230,54 @@
   </si>
   <si>
     <t>Remove Checked-In Status in Warehouse-In form</t>
+  </si>
+  <si>
+    <t>To be aligned as per the Process and not and alphabetic order</t>
+  </si>
+  <si>
+    <t>Commodity list to be provided for Masters</t>
+  </si>
+  <si>
+    <t>Venkat</t>
+  </si>
+  <si>
+    <t>Pre-Gatein (OTL, Lock &amp; Key, NIL)</t>
+  </si>
+  <si>
+    <t>To work on Shipper invoice currency</t>
+  </si>
+  <si>
+    <t>In Damage Check/Before Offloading change Quantity Deviation to Packages Deviation</t>
+  </si>
+  <si>
+    <t>In Damage Check/Before Offloading when Damages is not 'Nill Damage' or Quantity Devition or Ratification Process or Marks &amp; Numbers is 'No' then Status should be 'Hold'</t>
+  </si>
+  <si>
+    <t>Sridar Sir</t>
+  </si>
+  <si>
+    <t>Include camera option to upload the pics.</t>
+  </si>
+  <si>
+    <t>Fumigation Status - Inspection screen</t>
+  </si>
+  <si>
+    <t>Check Fumigation</t>
+  </si>
+  <si>
+    <t>In the inspection tab capture the weight and no of pacakages deviation</t>
+  </si>
+  <si>
+    <t>In Warehouse in tab check no of pieces is considered forstorage.</t>
+  </si>
+  <si>
+    <t>View option to be creasted for sridhar sir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSR </t>
+  </si>
+  <si>
+    <t>In storage report tab check the date formating for the check-out time</t>
   </si>
 </sst>
 </file>
@@ -1202,13 +1250,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
+      <selection pane="bottomRight" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2263,6 +2311,121 @@
       </c>
       <c r="H46" s="4"/>
     </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B54" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B55" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B56" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B57" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B58" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B60" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H45"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Latest update_Commit_12-Jan-23 - Jose
</commit_message>
<xml_diff>
--- a/Requirements/Requirments_v6.0.xlsx
+++ b/Requirements/Requirments_v6.0.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="95">
   <si>
     <t>Capture Commodity details - Add in Gate-In Form (Change Stock Type to Commodity Type) (Garments, Auto Parts, Leather Garments, Shoe Uppers, Finish Leather, Console, Electrical &amp; Electronics) - Jose (Venkat to send commodity details list)</t>
   </si>
@@ -278,6 +278,37 @@
   </si>
   <si>
     <t>In storage report tab check the date formating for the check-out time</t>
+  </si>
+  <si>
+    <t>Packing Type : Wooden Case, Carton Box, Ply wood. If wooden case : Fumigation to appear. Fumigation : Yes &amp; No. Yes to be completed. No : Customer or BVM (colour code). BVM : Date to be filled and accordingly.</t>
+  </si>
+  <si>
+    <t>Prakash</t>
+  </si>
+  <si>
+    <t>Empty truck photo to be in warehouse in tab</t>
+  </si>
+  <si>
+    <t>Dimension : Multiple line items to be clubbed</t>
+  </si>
+  <si>
+    <t>Multiple MAWB &amp; HAWB to be added</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency value should match invoice. So existing process holds good. </t>
+  </si>
+  <si>
+    <t>In warehousemaster rate form, bring customer short name in drop down</t>
+  </si>
+  <si>
+    <t>In Goods report form, headers are not alinged in with content. Check in similar forms as well.</t>
+  </si>
+  <si>
+    <t>Re-Order side Nave in WMS. 
+Pre-Gate In, Warehouse Jobs, Goods Report, Dispatch, Invoice, Reports, WMS Misc.</t>
   </si>
 </sst>
 </file>
@@ -1250,13 +1281,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B61" sqref="B61"/>
+      <selection pane="bottomRight" activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2312,119 +2343,392 @@
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="2">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="4"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="2">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="2">
+      <c r="D48" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="2">
+      <c r="C49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="2">
+      <c r="D50" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="2">
+      <c r="D51" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="2">
+      <c r="D52" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B54" s="1" t="s">
+      <c r="D53" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="3">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="1" t="s">
+      <c r="C54" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="3">
+        <v>54</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="B56" s="1" t="s">
+      <c r="C55" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A56" s="3">
+        <v>55</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="B57" s="1" t="s">
+      <c r="C56" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="3">
+        <v>56</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="1" t="s">
+      <c r="C57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E57" s="25">
+        <v>44937</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="3">
+        <v>57</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B59" s="1" t="s">
+      <c r="C58" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="3">
+        <v>58</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="B60" s="1" t="s">
+      <c r="D59" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="3">
+        <v>59</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>84</v>
       </c>
+      <c r="C60" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="25">
+        <v>44935</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A61" s="3">
+        <v>60</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61" s="25">
+        <v>44937</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="3">
+        <v>61</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D62" s="25">
+        <v>44937</v>
+      </c>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="3">
+        <v>62</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D63" s="25">
+        <v>44937</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
+        <v>63</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" s="25">
+        <v>44937</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="3">
+        <v>64</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="25">
+        <v>44938</v>
+      </c>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="3">
+        <v>65</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D66" s="25">
+        <v>44938</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="4"/>
+    </row>
+    <row r="67" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="3">
+        <v>66</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="25">
+        <v>44938</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H45"/>

</xml_diff>

<commit_message>
goods qty check Update_Commit_31-Jan-23-Jose
</commit_message>
<xml_diff>
--- a/Requirements/Requirments_v6.0.xlsx
+++ b/Requirements/Requirments_v6.0.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="155">
   <si>
     <t>Capture Commodity details - Add in Gate-In Form (Change Stock Type to Commodity Type) (Garments, Auto Parts, Leather Garments, Shoe Uppers, Finish Leather, Console, Electrical &amp; Electronics) - Jose (Venkat to send commodity details list)</t>
   </si>
@@ -487,6 +487,9 @@
   </si>
   <si>
     <t>Since pre-gatein number linked to multiple WH jobs, its not possible to remove from list.</t>
+  </si>
+  <si>
+    <t>In Inspection form, check-In weight and count throwing round off error</t>
   </si>
 </sst>
 </file>
@@ -1519,13 +1522,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I69" sqref="I69"/>
+      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3353,10 +3356,10 @@
       <c r="A78" s="3">
         <v>77</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D78" s="25">
@@ -3374,6 +3377,32 @@
       <c r="H78" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="3"/>
+      <c r="B79" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" s="25">
+        <v>44953</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F79" s="25">
+        <v>44953</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I79" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I69"/>

</xml_diff>

<commit_message>
wh goods mod file Update_Commit_23-Feb-23-Jose
</commit_message>
<xml_diff>
--- a/Requirements/Requirments_v6.0.xlsx
+++ b/Requirements/Requirments_v6.0.xlsx
@@ -17,14 +17,14 @@
     <sheet name="Project_Progress" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">req_text!$A$1:$J$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">req_text!$A$1:$J$119</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="208">
   <si>
     <t>Capture Commodity details - Add in Gate-In Form (Change Stock Type to Commodity Type) (Garments, Auto Parts, Leather Garments, Shoe Uppers, Finish Leather, Console, Electrical &amp; Electronics) - Jose (Venkat to send commodity details list)</t>
   </si>
@@ -599,6 +599,57 @@
   </si>
   <si>
     <t>In Vehicle master, change ICV to IDV</t>
+  </si>
+  <si>
+    <t>In Enquiry note add, aassigned to should be from login user</t>
+  </si>
+  <si>
+    <t>In Tripdetails add, include 'Biling Type' drop down. Vehicle Type Requested, Vehicle Type Placed</t>
+  </si>
+  <si>
+    <t>In Tripdetails add, change 'Vehicle Type' label to 'Vehicle Type Placed'.</t>
+  </si>
+  <si>
+    <t>In Tripdetails add, update driver name as drop down and pull license number, contact number from database</t>
+  </si>
+  <si>
+    <t>In Tripdetails add,From Location, To Location, Starting Km, Ending KM, Starting Date, Ending Date as seprate Row Items</t>
+  </si>
+  <si>
+    <t>In Consignment add, consigner, consignee,Consigner Invoice, Consigner Value, Value in INR, No of Pieces, weight to be added as separate line item</t>
+  </si>
+  <si>
+    <t>In Consignment add, move ebill no, date of Issue, Date of validity to trip details form</t>
+  </si>
+  <si>
+    <t>In Consignment add,remove 'Container' for 'Container Description' label.</t>
+  </si>
+  <si>
+    <t>In Consignment add,remove Dimension</t>
+  </si>
+  <si>
+    <t>In Consignment add,add 'Movement type' with FTL, LTL as drop down</t>
+  </si>
+  <si>
+    <t>In Consignment add,change 'Movement' to 'Consignent Type'</t>
+  </si>
+  <si>
+    <t>In Consignment note add, add customer code</t>
+  </si>
+  <si>
+    <t>In Consignment note add, add touch point between from and to</t>
+  </si>
+  <si>
+    <t>In Consignment add,add 'Freight Amount'</t>
+  </si>
+  <si>
+    <t>In Trip closure, change 'cost' in all labels to 'Charges'</t>
+  </si>
+  <si>
+    <t>In Trip closure, add 'Handling Charges and Halting Charges</t>
+  </si>
+  <si>
+    <t>In Trip closure, add customer ref no</t>
   </si>
 </sst>
 </file>
@@ -970,7 +1021,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1104,58 +1155,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -1178,37 +1177,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1256,7 +1224,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1271,19 +1239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1308,22 +1264,6 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1335,10 +1275,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1347,28 +1287,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1690,13 +1614,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F90" sqref="F90:F101"/>
+      <selection pane="bottomRight" activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1711,172 +1635,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="14">
         <v>44828</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14">
         <v>44927</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="13"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="14">
         <v>44828</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="15" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="9" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="14">
         <v>44828</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14">
         <v>44927</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="13"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="14">
         <v>44828</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="15" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="14">
         <v>44828</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14">
         <v>44927</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="13"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
@@ -1885,19 +1809,19 @@
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="14">
         <v>44828</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="11" t="s">
         <v>50</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -1911,23 +1835,23 @@
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="14">
         <v>44828</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14">
         <v>44927</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J8" s="4"/>
@@ -1939,23 +1863,23 @@
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="14">
         <v>44828</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18">
+      <c r="F9" s="14"/>
+      <c r="G9" s="14">
         <v>44927</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J9" s="4"/>
@@ -1967,19 +1891,19 @@
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="14">
         <v>44828</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J10" s="4"/>
@@ -1991,19 +1915,19 @@
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="14">
         <v>44828</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J11" s="4"/>
@@ -2015,19 +1939,19 @@
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="14">
         <v>44828</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J12" s="4"/>
@@ -2039,23 +1963,23 @@
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="C13" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="14">
         <v>44828</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18">
+      <c r="F13" s="14"/>
+      <c r="G13" s="14">
         <v>44927</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J13" s="4"/>
@@ -2067,19 +1991,19 @@
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="14">
         <v>44828</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="11" t="s">
         <v>50</v>
       </c>
       <c r="J14" s="5" t="s">
@@ -2093,19 +2017,19 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="14">
         <v>44828</v>
       </c>
-      <c r="F15" s="18"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J15" s="4"/>
@@ -2117,23 +2041,23 @@
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="14">
         <v>44828</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14">
         <v>44927</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J16" s="4"/>
@@ -2145,19 +2069,19 @@
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D17" s="11" t="s">
+      <c r="C17" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="14">
         <v>44828</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J17" s="4"/>
@@ -2169,23 +2093,23 @@
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D18" s="11" t="s">
+      <c r="C18" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="14">
         <v>44828</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18">
+      <c r="F18" s="14"/>
+      <c r="G18" s="14">
         <v>44927</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J18" s="4"/>
@@ -2197,23 +2121,23 @@
       <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="C19" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="14">
         <v>44828</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18">
+      <c r="F19" s="14"/>
+      <c r="G19" s="14">
         <v>44927</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J19" s="4"/>
@@ -2225,23 +2149,23 @@
       <c r="B20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="C20" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="14">
         <v>44828</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18">
+      <c r="F20" s="14"/>
+      <c r="G20" s="14">
         <v>44927</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J20" s="4"/>
@@ -2253,19 +2177,19 @@
       <c r="B21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="C21" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="14">
         <v>44828</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J21" s="4"/>
@@ -2277,19 +2201,19 @@
       <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D22" s="11" t="s">
+      <c r="C22" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="14">
         <v>44828</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J22" s="4"/>
@@ -2301,19 +2225,19 @@
       <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D23" s="11" t="s">
+      <c r="C23" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="14">
         <v>44828</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="16" t="s">
+      <c r="I23" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J23" s="4"/>
@@ -2325,23 +2249,23 @@
       <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="C24" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="14">
         <v>44828</v>
       </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18">
+      <c r="F24" s="14"/>
+      <c r="G24" s="14">
         <v>44927</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="I24" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J24" s="4"/>
@@ -2353,19 +2277,19 @@
       <c r="B25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D25" s="11" t="s">
+      <c r="C25" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="14">
         <v>44828</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="11" t="s">
         <v>50</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -2379,23 +2303,23 @@
       <c r="B26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="14">
         <v>44828</v>
       </c>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18">
+      <c r="F26" s="14"/>
+      <c r="G26" s="14">
         <v>44927</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J26" s="4"/>
@@ -2407,23 +2331,23 @@
       <c r="B27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="C27" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="14">
         <v>44828</v>
       </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18">
+      <c r="F27" s="14"/>
+      <c r="G27" s="14">
         <v>44927</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J27" s="4"/>
@@ -2435,19 +2359,19 @@
       <c r="B28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D28" s="11" t="s">
+      <c r="C28" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="14">
         <v>44828</v>
       </c>
-      <c r="F28" s="18"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="15" t="s">
+      <c r="I28" s="11" t="s">
         <v>50</v>
       </c>
       <c r="J28" s="5" t="s">
@@ -2461,23 +2385,23 @@
       <c r="B29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="C29" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="14">
         <v>44828</v>
       </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18">
+      <c r="F29" s="14"/>
+      <c r="G29" s="14">
         <v>44927</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J29" s="4"/>
@@ -2489,23 +2413,23 @@
       <c r="B30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D30" s="11" t="s">
+      <c r="C30" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="14">
         <v>44828</v>
       </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18">
+      <c r="F30" s="14"/>
+      <c r="G30" s="14">
         <v>44927</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J30" s="4"/>
@@ -2517,23 +2441,23 @@
       <c r="B31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" s="11" t="s">
+      <c r="C31" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="14">
         <v>44828</v>
       </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18">
+      <c r="F31" s="14"/>
+      <c r="G31" s="14">
         <v>44927</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J31" s="4"/>
@@ -2542,26 +2466,26 @@
       <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D32" s="11" t="s">
+      <c r="C32" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="14">
         <v>44828</v>
       </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18">
+      <c r="F32" s="14"/>
+      <c r="G32" s="14">
         <v>44927</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J32" s="5" t="s">
@@ -2572,26 +2496,26 @@
       <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D33" s="11" t="s">
+      <c r="C33" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="18">
+      <c r="E33" s="14">
         <v>44828</v>
       </c>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18">
+      <c r="F33" s="14"/>
+      <c r="G33" s="14">
         <v>44927</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H33" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J33" s="4"/>
@@ -2600,26 +2524,26 @@
       <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D34" s="11" t="s">
+      <c r="C34" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34" s="14">
         <v>44828</v>
       </c>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18">
+      <c r="F34" s="14"/>
+      <c r="G34" s="14">
         <v>44927</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="H34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I34" s="9" t="s">
+      <c r="I34" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J34" s="4"/>
@@ -2628,26 +2552,26 @@
       <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D35" s="11" t="s">
+      <c r="C35" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="14">
         <v>44828</v>
       </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18">
+      <c r="F35" s="14"/>
+      <c r="G35" s="14">
         <v>44927</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H35" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J35" s="4"/>
@@ -2656,26 +2580,26 @@
       <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="C36" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="14">
         <v>44828</v>
       </c>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18">
+      <c r="F36" s="14"/>
+      <c r="G36" s="14">
         <v>44927</v>
       </c>
-      <c r="H36" s="11" t="s">
+      <c r="H36" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I36" s="9" t="s">
+      <c r="I36" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J36" s="4"/>
@@ -2684,26 +2608,26 @@
       <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D37" s="11" t="s">
+      <c r="C37" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="14">
         <v>44828</v>
       </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18">
+      <c r="F37" s="14"/>
+      <c r="G37" s="14">
         <v>44927</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H37" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="I37" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J37" s="4"/>
@@ -2712,26 +2636,26 @@
       <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D38" s="11" t="s">
+      <c r="C38" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="14">
         <v>44828</v>
       </c>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18">
+      <c r="F38" s="14"/>
+      <c r="G38" s="14">
         <v>44927</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="H38" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J38" s="4"/>
@@ -2740,26 +2664,26 @@
       <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D39" s="11" t="s">
+      <c r="C39" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="14">
         <v>44828</v>
       </c>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18">
+      <c r="F39" s="14"/>
+      <c r="G39" s="14">
         <v>44927</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H39" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I39" s="9" t="s">
+      <c r="I39" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J39" s="5" t="s">
@@ -2770,22 +2694,22 @@
       <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="C40" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40" s="14">
         <v>44828</v>
       </c>
-      <c r="F40" s="18"/>
+      <c r="F40" s="14"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="15" t="s">
+      <c r="I40" s="11" t="s">
         <v>50</v>
       </c>
       <c r="J40" s="4" t="s">
@@ -2796,22 +2720,22 @@
       <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D41" s="11" t="s">
+      <c r="C41" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="14">
         <v>44828</v>
       </c>
-      <c r="F41" s="18"/>
+      <c r="F41" s="14"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="15" t="s">
+      <c r="I41" s="11" t="s">
         <v>50</v>
       </c>
       <c r="J41" s="5" t="s">
@@ -2822,22 +2746,22 @@
       <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D42" s="11" t="s">
+      <c r="C42" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="14">
         <v>44828</v>
       </c>
-      <c r="F42" s="18"/>
+      <c r="F42" s="14"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="I42" s="16" t="s">
+      <c r="I42" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J42" s="4"/>
@@ -2846,73 +2770,73 @@
       <c r="A43" s="3">
         <v>42</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D43" s="11" t="s">
+      <c r="C43" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="18">
+      <c r="E43" s="14">
         <v>44828</v>
       </c>
-      <c r="F43" s="18"/>
+      <c r="F43" s="14"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="16" t="s">
+      <c r="I43" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J43" s="4"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="19">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D44" s="20" t="s">
+      <c r="C44" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="21">
+      <c r="E44" s="14">
         <v>44828</v>
       </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="22" t="s">
+      <c r="F44" s="14"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="19">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D45" s="19" t="s">
+      <c r="C45" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E45" s="21">
+      <c r="E45" s="14">
         <v>44917</v>
       </c>
-      <c r="F45" s="21"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="J45" s="24"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
@@ -2921,19 +2845,19 @@
       <c r="B46" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E46" s="15">
         <v>44933</v>
       </c>
-      <c r="F46" s="25"/>
+      <c r="F46" s="15"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="3" t="s">
+      <c r="I46" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J46" s="4"/>
@@ -2945,19 +2869,19 @@
       <c r="B47" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E47" s="25">
+      <c r="E47" s="15">
         <v>44935</v>
       </c>
-      <c r="F47" s="25"/>
+      <c r="F47" s="15"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="3" t="s">
+      <c r="I47" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J47" s="4"/>
@@ -2969,19 +2893,19 @@
       <c r="B48" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E48" s="25">
+      <c r="E48" s="15">
         <v>44935</v>
       </c>
-      <c r="F48" s="25"/>
+      <c r="F48" s="15"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="3" t="s">
+      <c r="I48" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J48" s="4"/>
@@ -2993,19 +2917,19 @@
       <c r="B49" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E49" s="25">
+      <c r="E49" s="15">
         <v>44935</v>
       </c>
-      <c r="F49" s="25"/>
+      <c r="F49" s="15"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="3" t="s">
+      <c r="I49" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J49" s="4"/>
@@ -3017,19 +2941,19 @@
       <c r="B50" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E50" s="15">
         <v>44935</v>
       </c>
-      <c r="F50" s="25"/>
+      <c r="F50" s="15"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="27" t="s">
+      <c r="I50" s="17" t="s">
         <v>87</v>
       </c>
       <c r="J50" s="5" t="s">
@@ -3043,19 +2967,19 @@
       <c r="B51" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E51" s="15">
         <v>44935</v>
       </c>
-      <c r="F51" s="25"/>
+      <c r="F51" s="15"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="9" t="s">
+      <c r="I51" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J51" s="5" t="s">
@@ -3069,19 +2993,19 @@
       <c r="B52" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E52" s="15">
         <v>44935</v>
       </c>
-      <c r="F52" s="25"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="9" t="s">
+      <c r="I52" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J52" s="5" t="s">
@@ -3095,19 +3019,19 @@
       <c r="B53" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="15">
         <v>44935</v>
       </c>
-      <c r="F53" s="25"/>
+      <c r="F53" s="15"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="3" t="s">
+      <c r="I53" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J53" s="4"/>
@@ -3119,19 +3043,19 @@
       <c r="B54" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E54" s="15">
         <v>44935</v>
       </c>
-      <c r="F54" s="25"/>
+      <c r="F54" s="15"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="9" t="s">
+      <c r="I54" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J54" s="4"/>
@@ -3143,19 +3067,19 @@
       <c r="B55" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E55" s="25">
+      <c r="E55" s="15">
         <v>44935</v>
       </c>
-      <c r="F55" s="25"/>
+      <c r="F55" s="15"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="9" t="s">
+      <c r="I55" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J55" s="4"/>
@@ -3167,19 +3091,19 @@
       <c r="B56" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E56" s="25">
+      <c r="E56" s="15">
         <v>44935</v>
       </c>
-      <c r="F56" s="25"/>
+      <c r="F56" s="15"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="3" t="s">
+      <c r="I56" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J56" s="4"/>
@@ -3191,23 +3115,23 @@
       <c r="B57" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="25">
+      <c r="E57" s="15">
         <v>44935</v>
       </c>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25">
+      <c r="F57" s="15"/>
+      <c r="G57" s="15">
         <v>44937</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="9" t="s">
+      <c r="I57" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J57" s="4"/>
@@ -3219,19 +3143,19 @@
       <c r="B58" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E58" s="25">
+      <c r="E58" s="15">
         <v>44935</v>
       </c>
-      <c r="F58" s="25"/>
+      <c r="F58" s="15"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="3" t="s">
+      <c r="I58" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J58" s="4"/>
@@ -3243,19 +3167,19 @@
       <c r="B59" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E59" s="25">
+      <c r="E59" s="15">
         <v>44935</v>
       </c>
-      <c r="F59" s="25"/>
+      <c r="F59" s="15"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="3" t="s">
+      <c r="I59" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J59" s="4"/>
@@ -3267,25 +3191,25 @@
       <c r="B60" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E60" s="25">
+      <c r="E60" s="15">
         <v>44935</v>
       </c>
-      <c r="F60" s="25" t="s">
+      <c r="F60" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G60" s="25">
+      <c r="G60" s="15">
         <v>44940</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I60" s="9" t="s">
+      <c r="I60" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J60" s="4"/>
@@ -3297,25 +3221,25 @@
       <c r="B61" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E61" s="25">
+      <c r="E61" s="15">
         <v>44937</v>
       </c>
-      <c r="F61" s="25" t="s">
+      <c r="F61" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G61" s="25">
+      <c r="G61" s="15">
         <v>44940</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I61" s="9" t="s">
+      <c r="I61" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J61" s="4" t="s">
@@ -3329,19 +3253,19 @@
       <c r="B62" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E62" s="25">
+      <c r="E62" s="15">
         <v>44937</v>
       </c>
-      <c r="F62" s="25"/>
+      <c r="F62" s="15"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="I62" s="3" t="s">
+      <c r="I62" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J62" s="4"/>
@@ -3353,19 +3277,19 @@
       <c r="B63" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="25">
+      <c r="E63" s="15">
         <v>44937</v>
       </c>
-      <c r="F63" s="25"/>
+      <c r="F63" s="15"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="27" t="s">
+      <c r="I63" s="17" t="s">
         <v>87</v>
       </c>
       <c r="J63" s="5" t="s">
@@ -3379,19 +3303,19 @@
       <c r="B64" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E64" s="25">
+      <c r="E64" s="15">
         <v>44937</v>
       </c>
-      <c r="F64" s="25"/>
+      <c r="F64" s="15"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="3" t="s">
+      <c r="I64" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J64" s="4"/>
@@ -3403,19 +3327,19 @@
       <c r="B65" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C65" s="12" t="s">
+      <c r="C65" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E65" s="25">
+      <c r="E65" s="15">
         <v>44938</v>
       </c>
-      <c r="F65" s="25"/>
+      <c r="F65" s="15"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="3" t="s">
+      <c r="I65" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J65" s="4"/>
@@ -3427,19 +3351,19 @@
       <c r="B66" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E66" s="25">
+      <c r="E66" s="15">
         <v>44938</v>
       </c>
-      <c r="F66" s="25"/>
+      <c r="F66" s="15"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="26" t="s">
+      <c r="I66" s="16" t="s">
         <v>93</v>
       </c>
       <c r="J66" s="4"/>
@@ -3451,23 +3375,23 @@
       <c r="B67" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C67" s="12" t="s">
+      <c r="C67" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E67" s="25">
+      <c r="E67" s="15">
         <v>44938</v>
       </c>
-      <c r="F67" s="25"/>
-      <c r="G67" s="25">
+      <c r="F67" s="15"/>
+      <c r="G67" s="15">
         <v>44938</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I67" s="9" t="s">
+      <c r="I67" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J67" s="4"/>
@@ -3479,25 +3403,25 @@
       <c r="B68" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C68" s="12" t="s">
+      <c r="C68" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E68" s="25">
+      <c r="E68" s="15">
         <v>44938</v>
       </c>
-      <c r="F68" s="25" t="s">
+      <c r="F68" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G68" s="25">
+      <c r="G68" s="15">
         <v>44938</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I68" s="9" t="s">
+      <c r="I68" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J68" s="4"/>
@@ -3509,21 +3433,21 @@
       <c r="B69" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C69" s="12" t="s">
+      <c r="C69" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="25">
+      <c r="E69" s="15">
         <v>44939</v>
       </c>
-      <c r="F69" s="25" t="s">
+      <c r="F69" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
-      <c r="I69" s="27" t="s">
+      <c r="I69" s="17" t="s">
         <v>87</v>
       </c>
       <c r="J69" s="5" t="s">
@@ -3537,21 +3461,21 @@
       <c r="B70" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C70" s="12" t="s">
+      <c r="C70" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E70" s="25">
+      <c r="E70" s="15">
         <v>44940</v>
       </c>
-      <c r="F70" s="25" t="s">
+      <c r="F70" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="3" t="s">
+      <c r="I70" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J70" s="4"/>
@@ -3563,21 +3487,21 @@
       <c r="B71" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E71" s="25">
+      <c r="E71" s="15">
         <v>44940</v>
       </c>
-      <c r="F71" s="25" t="s">
+      <c r="F71" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
-      <c r="I71" s="3" t="s">
+      <c r="I71" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J71" s="4"/>
@@ -3589,21 +3513,21 @@
       <c r="B72" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C72" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E72" s="25">
+      <c r="E72" s="15">
         <v>44940</v>
       </c>
-      <c r="F72" s="25" t="s">
+      <c r="F72" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
-      <c r="I72" s="3" t="s">
+      <c r="I72" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J72" s="4"/>
@@ -3615,21 +3539,21 @@
       <c r="B73" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="12" t="s">
+      <c r="C73" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E73" s="25">
+      <c r="E73" s="15">
         <v>44944</v>
       </c>
-      <c r="F73" s="25" t="s">
+      <c r="F73" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="15" t="s">
+      <c r="I73" s="11" t="s">
         <v>50</v>
       </c>
       <c r="J73" s="4" t="s">
@@ -3643,25 +3567,25 @@
       <c r="B74" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C74" s="12" t="s">
+      <c r="C74" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E74" s="25">
+      <c r="E74" s="15">
         <v>44944</v>
       </c>
-      <c r="F74" s="25" t="s">
+      <c r="F74" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G74" s="25">
+      <c r="G74" s="15">
         <v>44945</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I74" s="9" t="s">
+      <c r="I74" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J74" s="4"/>
@@ -3673,25 +3597,25 @@
       <c r="B75" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C75" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E75" s="25">
+      <c r="E75" s="15">
         <v>44944</v>
       </c>
-      <c r="F75" s="25" t="s">
+      <c r="F75" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G75" s="25">
+      <c r="G75" s="15">
         <v>44951</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I75" s="9" t="s">
+      <c r="I75" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J75" s="4"/>
@@ -3703,25 +3627,25 @@
       <c r="B76" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C76" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E76" s="25">
+      <c r="E76" s="15">
         <v>44944</v>
       </c>
-      <c r="F76" s="25" t="s">
+      <c r="F76" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G76" s="25">
+      <c r="G76" s="15">
         <v>44944</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I76" s="9" t="s">
+      <c r="I76" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J76" s="4"/>
@@ -3733,21 +3657,21 @@
       <c r="B77" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E77" s="25">
+      <c r="E77" s="15">
         <v>44944</v>
       </c>
-      <c r="F77" s="25" t="s">
+      <c r="F77" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="3" t="s">
+      <c r="I77" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J77" s="4"/>
@@ -3759,25 +3683,25 @@
       <c r="B78" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C78" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="25">
+      <c r="E78" s="15">
         <v>44951</v>
       </c>
-      <c r="F78" s="25" t="s">
+      <c r="F78" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G78" s="25">
+      <c r="G78" s="15">
         <v>44951</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I78" s="9" t="s">
+      <c r="I78" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J78" s="4"/>
@@ -3789,25 +3713,25 @@
       <c r="B79" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C79" s="12" t="s">
+      <c r="C79" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E79" s="25">
+      <c r="E79" s="15">
         <v>44953</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G79" s="25">
+      <c r="G79" s="15">
         <v>44953</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I79" s="9" t="s">
+      <c r="I79" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J79" s="4"/>
@@ -3819,25 +3743,25 @@
       <c r="B80" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C80" s="12" t="s">
+      <c r="C80" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E80" s="25">
+      <c r="E80" s="15">
         <v>44956</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G80" s="25">
+      <c r="G80" s="15">
         <v>44957</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I80" s="9" t="s">
+      <c r="I80" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J80" s="4"/>
@@ -3849,25 +3773,25 @@
       <c r="B81" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="C81" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E81" s="25">
+      <c r="E81" s="15">
         <v>44956</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G81" s="25">
+      <c r="G81" s="15">
         <v>44957</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I81" s="9" t="s">
+      <c r="I81" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J81" s="4"/>
@@ -3879,13 +3803,13 @@
       <c r="B82" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C82" s="12" t="s">
+      <c r="C82" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E82" s="25">
+      <c r="E82" s="15">
         <v>44960</v>
       </c>
       <c r="F82" s="3" t="s">
@@ -3893,7 +3817,7 @@
       </c>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
-      <c r="I82" s="3" t="s">
+      <c r="I82" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J82" s="4" t="s">
@@ -3907,13 +3831,13 @@
       <c r="B83" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C83" s="12" t="s">
+      <c r="C83" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E83" s="25">
+      <c r="E83" s="15">
         <v>44960</v>
       </c>
       <c r="F83" s="3" t="s">
@@ -3921,7 +3845,7 @@
       </c>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
-      <c r="I83" s="3" t="s">
+      <c r="I83" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J83" s="4" t="s">
@@ -3935,25 +3859,25 @@
       <c r="B84" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C84" s="12" t="s">
+      <c r="C84" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E84" s="25">
+      <c r="E84" s="15">
         <v>44960</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="25">
+      <c r="G84" s="15">
         <v>44968</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I84" s="9" t="s">
+      <c r="I84" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J84" s="4" t="s">
@@ -3967,13 +3891,13 @@
       <c r="B85" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C85" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E85" s="25">
+      <c r="E85" s="15">
         <v>44960</v>
       </c>
       <c r="F85" s="3" t="s">
@@ -3981,7 +3905,7 @@
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="3" t="s">
+      <c r="I85" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J85" s="4" t="s">
@@ -3995,13 +3919,13 @@
       <c r="B86" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C86" s="12" t="s">
+      <c r="C86" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E86" s="25">
+      <c r="E86" s="15">
         <v>44960</v>
       </c>
       <c r="F86" s="3" t="s">
@@ -4009,7 +3933,7 @@
       </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
-      <c r="I86" s="3" t="s">
+      <c r="I86" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J86" s="4" t="s">
@@ -4023,13 +3947,13 @@
       <c r="B87" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C87" s="12" t="s">
+      <c r="C87" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E87" s="25">
+      <c r="E87" s="15">
         <v>44960</v>
       </c>
       <c r="F87" s="3" t="s">
@@ -4037,7 +3961,7 @@
       </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
-      <c r="I87" s="3" t="s">
+      <c r="I87" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J87" s="4" t="s">
@@ -4051,13 +3975,13 @@
       <c r="B88" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C88" s="12" t="s">
+      <c r="C88" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E88" s="25">
+      <c r="E88" s="15">
         <v>44960</v>
       </c>
       <c r="F88" s="3" t="s">
@@ -4065,40 +3989,40 @@
       </c>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
-      <c r="I88" s="3" t="s">
+      <c r="I88" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J88" s="4"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A89" s="35">
+      <c r="A89" s="3">
         <v>88</v>
       </c>
-      <c r="B89" s="36" t="s">
+      <c r="B89" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C89" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="D89" s="38" t="s">
+      <c r="C89" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E89" s="39">
+      <c r="E89" s="15">
         <v>44973</v>
       </c>
-      <c r="F89" s="35" t="s">
+      <c r="F89" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G89" s="39">
+      <c r="G89" s="15">
         <v>44973</v>
       </c>
-      <c r="H89" s="38" t="s">
+      <c r="H89" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I89" s="40" t="s">
+      <c r="I89" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J89" s="41"/>
+      <c r="J89" s="4"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
@@ -4107,21 +4031,21 @@
       <c r="B90" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C90" s="12" t="s">
+      <c r="C90" s="8" t="s">
         <v>166</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E90" s="25">
+      <c r="E90" s="15">
         <v>44975</v>
       </c>
-      <c r="F90" s="25" t="s">
+      <c r="F90" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
-      <c r="I90" s="3" t="s">
+      <c r="I90" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J90" s="4"/>
@@ -4139,15 +4063,15 @@
       <c r="D91" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E91" s="25">
+      <c r="E91" s="15">
         <v>44975</v>
       </c>
-      <c r="F91" s="25" t="s">
+      <c r="F91" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
-      <c r="I91" s="3" t="s">
+      <c r="I91" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J91" s="4"/>
@@ -4165,19 +4089,19 @@
       <c r="D92" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E92" s="25">
+      <c r="E92" s="15">
         <v>44975</v>
       </c>
-      <c r="F92" s="25" t="s">
+      <c r="F92" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G92" s="25">
+      <c r="G92" s="15">
         <v>44975</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I92" s="9" t="s">
+      <c r="I92" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J92" s="4"/>
@@ -4195,19 +4119,19 @@
       <c r="D93" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E93" s="25">
+      <c r="E93" s="15">
         <v>44975</v>
       </c>
-      <c r="F93" s="25" t="s">
+      <c r="F93" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G93" s="25">
+      <c r="G93" s="15">
         <v>44975</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I93" s="9" t="s">
+      <c r="I93" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J93" s="4"/>
@@ -4225,15 +4149,15 @@
       <c r="D94" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E94" s="25">
+      <c r="E94" s="15">
         <v>44975</v>
       </c>
-      <c r="F94" s="25" t="s">
+      <c r="F94" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
-      <c r="I94" s="3" t="s">
+      <c r="I94" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J94" s="4"/>
@@ -4251,15 +4175,15 @@
       <c r="D95" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E95" s="25">
+      <c r="E95" s="15">
         <v>44975</v>
       </c>
-      <c r="F95" s="25" t="s">
+      <c r="F95" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
-      <c r="I95" s="3" t="s">
+      <c r="I95" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J95" s="4"/>
@@ -4277,15 +4201,15 @@
       <c r="D96" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E96" s="25">
+      <c r="E96" s="15">
         <v>44975</v>
       </c>
-      <c r="F96" s="25" t="s">
+      <c r="F96" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-      <c r="I96" s="3" t="s">
+      <c r="I96" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J96" s="4"/>
@@ -4303,15 +4227,15 @@
       <c r="D97" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E97" s="25">
+      <c r="E97" s="15">
         <v>44975</v>
       </c>
-      <c r="F97" s="25" t="s">
+      <c r="F97" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
-      <c r="I97" s="3" t="s">
+      <c r="I97" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J97" s="4"/>
@@ -4329,15 +4253,15 @@
       <c r="D98" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E98" s="25">
+      <c r="E98" s="15">
         <v>44975</v>
       </c>
-      <c r="F98" s="25" t="s">
+      <c r="F98" s="15" t="s">
         <v>111</v>
       </c>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
-      <c r="I98" s="3" t="s">
+      <c r="I98" s="12" t="s">
         <v>48</v>
       </c>
       <c r="J98" s="4"/>
@@ -4355,19 +4279,19 @@
       <c r="D99" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E99" s="25">
+      <c r="E99" s="15">
         <v>44975</v>
       </c>
-      <c r="F99" s="25" t="s">
+      <c r="F99" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G99" s="25">
+      <c r="G99" s="15">
         <v>44975</v>
       </c>
       <c r="H99" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I99" s="9" t="s">
+      <c r="I99" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J99" s="4"/>
@@ -4376,27 +4300,33 @@
       <c r="A100" s="3">
         <v>99</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="5" t="s">
         <v>187</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D100" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E100" s="25">
+      <c r="E100" s="15">
         <v>44975</v>
       </c>
-      <c r="F100" s="25" t="s">
+      <c r="F100" s="15" t="s">
         <v>111</v>
       </c>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J100" s="4"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>100</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="5" t="s">
         <v>190</v>
       </c>
       <c r="C101" s="5" t="s">
@@ -4405,24 +4335,493 @@
       <c r="D101" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E101" s="25">
+      <c r="E101" s="15">
         <v>44975</v>
       </c>
-      <c r="F101" s="25" t="s">
+      <c r="F101" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G101" s="25">
+      <c r="G101" s="15">
         <v>44975</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I101" s="9" t="s">
+      <c r="I101" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="J101" s="4"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="3">
+        <v>101</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E102" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F102" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J102" s="4"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103" s="3">
+        <v>102</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E103" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F103" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J103" s="4"/>
+    </row>
+    <row r="104" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A104" s="3">
+        <v>103</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E104" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F104" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J104" s="4"/>
+    </row>
+    <row r="105" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A105" s="3">
+        <v>104</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E105" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F105" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J105" s="4"/>
+    </row>
+    <row r="106" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A106" s="3">
+        <v>105</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E106" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F106" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J106" s="4"/>
+    </row>
+    <row r="107" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A107" s="3">
+        <v>106</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E107" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F107" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+      <c r="I107" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J107" s="4"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108" s="3">
+        <v>107</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E108" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F108" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J108" s="4"/>
+    </row>
+    <row r="109" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A109" s="3">
+        <v>108</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E109" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F109" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J109" s="4"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A110" s="3">
+        <v>109</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E110" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F110" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
+      <c r="I110" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J110" s="4"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A111" s="3">
+        <v>110</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E111" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F111" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+      <c r="I111" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J111" s="4"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A112" s="3">
+        <v>111</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E112" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F112" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J112" s="4"/>
+    </row>
+    <row r="113" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A113" s="3">
+        <v>112</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E113" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F113" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+      <c r="I113" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J113" s="4"/>
+    </row>
+    <row r="114" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A114" s="3">
+        <v>113</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E114" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F114" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G114" s="3"/>
+      <c r="H114" s="3"/>
+      <c r="I114" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J114" s="4"/>
+    </row>
+    <row r="115" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A115" s="3">
+        <v>114</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E115" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F115" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
+      <c r="I115" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J115" s="4"/>
+    </row>
+    <row r="116" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A116" s="3">
+        <v>115</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E116" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F116" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3"/>
+      <c r="I116" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J116" s="4"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A117" s="3">
+        <v>116</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E117" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F117" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
+      <c r="I117" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J117" s="4"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A118" s="3">
+        <v>117</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E118" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F118" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3"/>
+      <c r="I118" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J118" s="4"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A119" s="3">
+        <v>118</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E119" s="15">
+        <v>44978</v>
+      </c>
+      <c r="F119" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G119" s="3"/>
+      <c r="H119" s="3"/>
+      <c r="I119" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J119" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J69"/>
+  <autoFilter ref="A1:J119"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4459,68 +4858,68 @@
     <col min="21" max="21" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:21" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="21" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4590,7 +4989,7 @@
       <c r="I3" t="s">
         <v>140</v>
       </c>
-      <c r="N3" s="29">
+      <c r="N3" s="19">
         <v>0.18</v>
       </c>
       <c r="R3" t="s">
@@ -4631,55 +5030,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="23" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32">
+    <row r="2" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22">
         <v>0.9</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="22">
         <v>0.6</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="22">
         <v>0</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="22">
         <v>0</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="22">
         <v>0.7</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="22">
         <v>0</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="22">
         <v>0.7</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H2" s="22">
         <v>0.8</v>
       </c>
     </row>

</xml_diff>